<commit_message>
Created a file structure for the test cases.
</commit_message>
<xml_diff>
--- a/candidate_data.xlsx
+++ b/candidate_data.xlsx
@@ -20,124 +20,124 @@
     <t>candidatePhoneNumber</t>
   </si>
   <si>
+    <t>Anil</t>
+  </si>
+  <si>
+    <t>9174553393</t>
+  </si>
+  <si>
+    <t>Pushpendra</t>
+  </si>
+  <si>
+    <t>9838356619</t>
+  </si>
+  <si>
+    <t>9620501927</t>
+  </si>
+  <si>
     <t>Mahaveer</t>
   </si>
   <si>
-    <t>9499475074</t>
+    <t>9767302767</t>
+  </si>
+  <si>
+    <t>9994288961</t>
   </si>
   <si>
     <t>Kapil</t>
   </si>
   <si>
-    <t>9737518952</t>
+    <t>9185240011</t>
+  </si>
+  <si>
+    <t>Niranjan</t>
+  </si>
+  <si>
+    <t>9915641545</t>
+  </si>
+  <si>
+    <t>9411102267</t>
+  </si>
+  <si>
+    <t>Himmat</t>
+  </si>
+  <si>
+    <t>9394199983</t>
+  </si>
+  <si>
+    <t>9308693396</t>
+  </si>
+  <si>
+    <t>9605456238</t>
+  </si>
+  <si>
+    <t>9522220048</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>9233730316</t>
+  </si>
+  <si>
+    <t>Pavan</t>
+  </si>
+  <si>
+    <t>9974306980</t>
+  </si>
+  <si>
+    <t>9442361280</t>
+  </si>
+  <si>
+    <t>9667493230</t>
+  </si>
+  <si>
+    <t>9913511085</t>
+  </si>
+  <si>
+    <t>9412799818</t>
+  </si>
+  <si>
+    <t>Lakshpat</t>
+  </si>
+  <si>
+    <t>9285508813</t>
+  </si>
+  <si>
+    <t>9974783093</t>
+  </si>
+  <si>
+    <t>9728494689</t>
+  </si>
+  <si>
+    <t>9602290372</t>
+  </si>
+  <si>
+    <t>9373931892</t>
+  </si>
+  <si>
+    <t>9704522328</t>
+  </si>
+  <si>
+    <t>9643336175</t>
+  </si>
+  <si>
+    <t>9878563640</t>
+  </si>
+  <si>
+    <t>9919290003</t>
   </si>
   <si>
     <t>Shahrukh</t>
   </si>
   <si>
-    <t>9893752972</t>
-  </si>
-  <si>
-    <t>Anil</t>
-  </si>
-  <si>
-    <t>9866401386</t>
-  </si>
-  <si>
-    <t>Pavan</t>
-  </si>
-  <si>
-    <t>9501975998</t>
-  </si>
-  <si>
-    <t>9858592897</t>
-  </si>
-  <si>
-    <t>Himmat</t>
-  </si>
-  <si>
-    <t>9568558980</t>
-  </si>
-  <si>
-    <t>Niranjan</t>
-  </si>
-  <si>
-    <t>9991681005</t>
-  </si>
-  <si>
-    <t>9535583142</t>
-  </si>
-  <si>
-    <t>9784419012</t>
-  </si>
-  <si>
-    <t>Pushpendra</t>
-  </si>
-  <si>
-    <t>9659042486</t>
-  </si>
-  <si>
-    <t>9999753716</t>
-  </si>
-  <si>
-    <t>9239003906</t>
-  </si>
-  <si>
-    <t>9913796045</t>
-  </si>
-  <si>
-    <t>9684565334</t>
-  </si>
-  <si>
-    <t>9132378115</t>
-  </si>
-  <si>
-    <t>9339798226</t>
-  </si>
-  <si>
-    <t>9789997260</t>
-  </si>
-  <si>
-    <t>9397316924</t>
-  </si>
-  <si>
-    <t>9648390404</t>
-  </si>
-  <si>
-    <t>9914202222</t>
-  </si>
-  <si>
-    <t>9393250484</t>
-  </si>
-  <si>
-    <t>9379433025</t>
-  </si>
-  <si>
-    <t>9474451705</t>
-  </si>
-  <si>
-    <t>9555233901</t>
-  </si>
-  <si>
-    <t>9541551128</t>
-  </si>
-  <si>
-    <t>Ram</t>
-  </si>
-  <si>
-    <t>9780691873</t>
-  </si>
-  <si>
-    <t>Lakshpat</t>
-  </si>
-  <si>
-    <t>9489358968</t>
-  </si>
-  <si>
-    <t>9810020069</t>
-  </si>
-  <si>
-    <t>9797720677</t>
+    <t>9219556116</t>
+  </si>
+  <si>
+    <t>9558782117</t>
+  </si>
+  <si>
+    <t>9164567643</t>
   </si>
 </sst>
 </file>
@@ -214,95 +214,95 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>6</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s" s="0">
         <v>8</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s" s="0">
         <v>13</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s" s="0">
         <v>19</v>
-      </c>
-      <c r="B13" t="s" s="0">
-        <v>21</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s" s="0">
         <v>23</v>
@@ -310,7 +310,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s" s="0">
         <v>24</v>
@@ -318,7 +318,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s" s="0">
         <v>25</v>
@@ -326,7 +326,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s" s="0">
         <v>26</v>
@@ -334,7 +334,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s" s="0">
         <v>27</v>
@@ -342,71 +342,71 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="B28" t="s" s="0">
         <v>37</v>
@@ -422,7 +422,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B30" t="s" s="0">
         <v>40</v>
@@ -430,7 +430,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="B31" t="s" s="0">
         <v>41</v>

</xml_diff>

<commit_message>
Added more cases in Bulk Upload TestCases
</commit_message>
<xml_diff>
--- a/candidate_data.xlsx
+++ b/candidate_data.xlsx
@@ -20,124 +20,124 @@
     <t>candidatePhoneNumber</t>
   </si>
   <si>
+    <t>Himmat</t>
+  </si>
+  <si>
+    <t>9415871487</t>
+  </si>
+  <si>
+    <t>Pushpendra</t>
+  </si>
+  <si>
+    <t>9979648308</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>9667420774</t>
+  </si>
+  <si>
+    <t>Pavan</t>
+  </si>
+  <si>
+    <t>9755684380</t>
+  </si>
+  <si>
+    <t>9383546126</t>
+  </si>
+  <si>
+    <t>9771899012</t>
+  </si>
+  <si>
+    <t>9737279612</t>
+  </si>
+  <si>
+    <t>Kapil</t>
+  </si>
+  <si>
+    <t>9990507173</t>
+  </si>
+  <si>
+    <t>9711590112</t>
+  </si>
+  <si>
+    <t>9238033180</t>
+  </si>
+  <si>
+    <t>9543298009</t>
+  </si>
+  <si>
+    <t>Lakshpat</t>
+  </si>
+  <si>
+    <t>9646093643</t>
+  </si>
+  <si>
+    <t>9304781015</t>
+  </si>
+  <si>
+    <t>9649495450</t>
+  </si>
+  <si>
+    <t>Mahaveer</t>
+  </si>
+  <si>
+    <t>9665104273</t>
+  </si>
+  <si>
+    <t>9825890317</t>
+  </si>
+  <si>
+    <t>9654375920</t>
+  </si>
+  <si>
     <t>Anil</t>
   </si>
   <si>
-    <t>9174553393</t>
-  </si>
-  <si>
-    <t>Pushpendra</t>
-  </si>
-  <si>
-    <t>9838356619</t>
-  </si>
-  <si>
-    <t>9620501927</t>
-  </si>
-  <si>
-    <t>Mahaveer</t>
-  </si>
-  <si>
-    <t>9767302767</t>
-  </si>
-  <si>
-    <t>9994288961</t>
-  </si>
-  <si>
-    <t>Kapil</t>
-  </si>
-  <si>
-    <t>9185240011</t>
+    <t>9921903521</t>
+  </si>
+  <si>
+    <t>9273571514</t>
   </si>
   <si>
     <t>Niranjan</t>
   </si>
   <si>
-    <t>9915641545</t>
-  </si>
-  <si>
-    <t>9411102267</t>
-  </si>
-  <si>
-    <t>Himmat</t>
-  </si>
-  <si>
-    <t>9394199983</t>
-  </si>
-  <si>
-    <t>9308693396</t>
-  </si>
-  <si>
-    <t>9605456238</t>
-  </si>
-  <si>
-    <t>9522220048</t>
-  </si>
-  <si>
-    <t>Ram</t>
-  </si>
-  <si>
-    <t>9233730316</t>
-  </si>
-  <si>
-    <t>Pavan</t>
-  </si>
-  <si>
-    <t>9974306980</t>
-  </si>
-  <si>
-    <t>9442361280</t>
-  </si>
-  <si>
-    <t>9667493230</t>
-  </si>
-  <si>
-    <t>9913511085</t>
-  </si>
-  <si>
-    <t>9412799818</t>
-  </si>
-  <si>
-    <t>Lakshpat</t>
-  </si>
-  <si>
-    <t>9285508813</t>
-  </si>
-  <si>
-    <t>9974783093</t>
-  </si>
-  <si>
-    <t>9728494689</t>
-  </si>
-  <si>
-    <t>9602290372</t>
-  </si>
-  <si>
-    <t>9373931892</t>
-  </si>
-  <si>
-    <t>9704522328</t>
-  </si>
-  <si>
-    <t>9643336175</t>
-  </si>
-  <si>
-    <t>9878563640</t>
-  </si>
-  <si>
-    <t>9919290003</t>
+    <t>9886049878</t>
+  </si>
+  <si>
+    <t>9310031079</t>
   </si>
   <si>
     <t>Shahrukh</t>
   </si>
   <si>
-    <t>9219556116</t>
-  </si>
-  <si>
-    <t>9558782117</t>
-  </si>
-  <si>
-    <t>9164567643</t>
+    <t>9780419283</t>
+  </si>
+  <si>
+    <t>9933544778</t>
+  </si>
+  <si>
+    <t>9418008206</t>
+  </si>
+  <si>
+    <t>9694025993</t>
+  </si>
+  <si>
+    <t>9634676230</t>
+  </si>
+  <si>
+    <t>9705491742</t>
+  </si>
+  <si>
+    <t>9505609423</t>
+  </si>
+  <si>
+    <t>9285859744</t>
+  </si>
+  <si>
+    <t>9345574942</t>
   </si>
 </sst>
 </file>
@@ -214,31 +214,31 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s" s="0">
         <v>11</v>
@@ -246,15 +246,15 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s" s="0">
         <v>12</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>13</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s" s="0">
         <v>14</v>
@@ -262,31 +262,31 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s" s="0">
         <v>15</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>16</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s" s="0">
         <v>19</v>
@@ -294,47 +294,47 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s" s="0">
         <v>20</v>
-      </c>
-      <c r="B14" t="s" s="0">
-        <v>21</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s" s="0">
         <v>27</v>
@@ -342,15 +342,15 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s" s="0">
         <v>28</v>
-      </c>
-      <c r="B20" t="s" s="0">
-        <v>29</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s" s="0">
         <v>30</v>
@@ -358,7 +358,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B22" t="s" s="0">
         <v>31</v>
@@ -366,55 +366,55 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="B29" t="s" s="0">
         <v>39</v>
@@ -422,7 +422,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s" s="0">
         <v>40</v>
@@ -430,7 +430,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s" s="0">
         <v>41</v>

</xml_diff>

<commit_message>
Added code to verify Dowmload candidate status file
</commit_message>
<xml_diff>
--- a/candidate_data.xlsx
+++ b/candidate_data.xlsx
@@ -20,124 +20,124 @@
     <t>candidatePhoneNumber</t>
   </si>
   <si>
+    <t>Mahaveer</t>
+  </si>
+  <si>
+    <t>9820986663</t>
+  </si>
+  <si>
+    <t>9298235707</t>
+  </si>
+  <si>
+    <t>Anil</t>
+  </si>
+  <si>
+    <t>9526639140</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>9242017157</t>
+  </si>
+  <si>
+    <t>9911309444</t>
+  </si>
+  <si>
+    <t>Niranjan</t>
+  </si>
+  <si>
+    <t>9329062784</t>
+  </si>
+  <si>
+    <t>9595618726</t>
+  </si>
+  <si>
+    <t>Kapil</t>
+  </si>
+  <si>
+    <t>9353058247</t>
+  </si>
+  <si>
+    <t>Pavan</t>
+  </si>
+  <si>
+    <t>9360394595</t>
+  </si>
+  <si>
     <t>Himmat</t>
   </si>
   <si>
-    <t>9415871487</t>
+    <t>9156947891</t>
   </si>
   <si>
     <t>Pushpendra</t>
   </si>
   <si>
-    <t>9979648308</t>
-  </si>
-  <si>
-    <t>Ram</t>
-  </si>
-  <si>
-    <t>9667420774</t>
-  </si>
-  <si>
-    <t>Pavan</t>
-  </si>
-  <si>
-    <t>9755684380</t>
-  </si>
-  <si>
-    <t>9383546126</t>
-  </si>
-  <si>
-    <t>9771899012</t>
-  </si>
-  <si>
-    <t>9737279612</t>
-  </si>
-  <si>
-    <t>Kapil</t>
-  </si>
-  <si>
-    <t>9990507173</t>
-  </si>
-  <si>
-    <t>9711590112</t>
-  </si>
-  <si>
-    <t>9238033180</t>
-  </si>
-  <si>
-    <t>9543298009</t>
+    <t>9103976836</t>
+  </si>
+  <si>
+    <t>9387530958</t>
+  </si>
+  <si>
+    <t>9324306568</t>
+  </si>
+  <si>
+    <t>9126988095</t>
+  </si>
+  <si>
+    <t>Shahrukh</t>
+  </si>
+  <si>
+    <t>9191088222</t>
+  </si>
+  <si>
+    <t>9862777691</t>
+  </si>
+  <si>
+    <t>9242592392</t>
+  </si>
+  <si>
+    <t>9202122694</t>
+  </si>
+  <si>
+    <t>9254482831</t>
+  </si>
+  <si>
+    <t>9761405548</t>
+  </si>
+  <si>
+    <t>9450437865</t>
+  </si>
+  <si>
+    <t>9515933278</t>
+  </si>
+  <si>
+    <t>9400719871</t>
   </si>
   <si>
     <t>Lakshpat</t>
   </si>
   <si>
-    <t>9646093643</t>
-  </si>
-  <si>
-    <t>9304781015</t>
-  </si>
-  <si>
-    <t>9649495450</t>
-  </si>
-  <si>
-    <t>Mahaveer</t>
-  </si>
-  <si>
-    <t>9665104273</t>
-  </si>
-  <si>
-    <t>9825890317</t>
-  </si>
-  <si>
-    <t>9654375920</t>
-  </si>
-  <si>
-    <t>Anil</t>
-  </si>
-  <si>
-    <t>9921903521</t>
-  </si>
-  <si>
-    <t>9273571514</t>
-  </si>
-  <si>
-    <t>Niranjan</t>
-  </si>
-  <si>
-    <t>9886049878</t>
-  </si>
-  <si>
-    <t>9310031079</t>
-  </si>
-  <si>
-    <t>Shahrukh</t>
-  </si>
-  <si>
-    <t>9780419283</t>
-  </si>
-  <si>
-    <t>9933544778</t>
-  </si>
-  <si>
-    <t>9418008206</t>
-  </si>
-  <si>
-    <t>9694025993</t>
-  </si>
-  <si>
-    <t>9634676230</t>
-  </si>
-  <si>
-    <t>9705491742</t>
-  </si>
-  <si>
-    <t>9505609423</t>
-  </si>
-  <si>
-    <t>9285859744</t>
-  </si>
-  <si>
-    <t>9345574942</t>
+    <t>9577789344</t>
+  </si>
+  <si>
+    <t>9528180613</t>
+  </si>
+  <si>
+    <t>9329928614</t>
+  </si>
+  <si>
+    <t>9941782744</t>
+  </si>
+  <si>
+    <t>9481176081</t>
+  </si>
+  <si>
+    <t>9485294768</t>
+  </si>
+  <si>
+    <t>9602742343</t>
   </si>
 </sst>
 </file>
@@ -206,39 +206,39 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="0">
         <v>4</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>6</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s" s="0">
         <v>8</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s" s="0">
         <v>11</v>
@@ -246,7 +246,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s" s="0">
         <v>12</v>
@@ -262,95 +262,95 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s" s="0">
         <v>30</v>
@@ -366,23 +366,23 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s" s="0">
         <v>32</v>
-      </c>
-      <c r="B23" t="s" s="0">
-        <v>33</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s" s="0">
         <v>35</v>
@@ -390,7 +390,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s" s="0">
         <v>36</v>
@@ -398,7 +398,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s" s="0">
         <v>37</v>
@@ -406,7 +406,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s" s="0">
         <v>38</v>
@@ -414,7 +414,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B29" t="s" s="0">
         <v>39</v>
@@ -422,7 +422,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s" s="0">
         <v>40</v>
@@ -430,7 +430,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s" s="0">
         <v>41</v>

</xml_diff>